<commit_message>
Job Done Final Touches Left--force
</commit_message>
<xml_diff>
--- a/Hostel Allocation Grouping (Responses).xlsx
+++ b/Hostel Allocation Grouping (Responses).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bikra\Desktop\Programming projects\Python\Google Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D5DA48-FF8C-4AA8-9066-0C6437881331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A66BC4-46A8-4A0F-BC6B-0B2BEDF46797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -408,7 +408,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -638,12 +638,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{177318D8-E89B-4B7C-9D0F-52B70A6451BB}"/>
-    <hyperlink ref="B8" r:id="rId2" xr:uid="{A6D76BD6-6AF0-430E-B32D-0D3BBDAF88D8}"/>
-    <hyperlink ref="B6" r:id="rId3" xr:uid="{311F4EEB-BBCF-4F75-8098-1485191BBEE9}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{F9AAAE9C-F6AA-4E4D-B35D-047BF7383622}"/>
-    <hyperlink ref="B7" r:id="rId5" xr:uid="{D09B4EB2-24BB-44C8-9D46-DE1CCA595FBE}"/>
-    <hyperlink ref="B2" r:id="rId6" xr:uid="{4D0A1B75-9E31-4F28-9ACB-FC17CB4EE31A}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{4D0A1B75-9E31-4F28-9ACB-FC17CB4EE31A}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{D09B4EB2-24BB-44C8-9D46-DE1CCA595FBE}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{F9AAAE9C-F6AA-4E4D-B35D-047BF7383622}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{311F4EEB-BBCF-4F75-8098-1485191BBEE9}"/>
+    <hyperlink ref="B8" r:id="rId5" xr:uid="{A6D76BD6-6AF0-430E-B32D-0D3BBDAF88D8}"/>
+    <hyperlink ref="B3" r:id="rId6" xr:uid="{177318D8-E89B-4B7C-9D0F-52B70A6451BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>